<commit_message>
Inclusion of expanded encounters and inclusion of elements within cells
</commit_message>
<xml_diff>
--- a/Deliverables/IG/examples/cycles_1.xlsx
+++ b/Deliverables/IG/examples/cycles_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94A8E21-A165-9748-90F6-CE312FECE3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F713249-7440-2544-B38D-496EFE4063AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43740" yWindow="2500" windowWidth="33600" windowHeight="19480" activeTab="2" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="31140" yWindow="7000" windowWidth="33600" windowHeight="19480" activeTab="2" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,9 @@
     <sheet name="studyDesignOE" sheetId="7" r:id="rId7"/>
     <sheet name="studyDesignEstimands" sheetId="9" r:id="rId8"/>
     <sheet name="studyDesignProcedures" sheetId="11" r:id="rId9"/>
-    <sheet name="configuration" sheetId="10" r:id="rId10"/>
+    <sheet name="studyDesignEncounters" sheetId="12" r:id="rId10"/>
+    <sheet name="studyDesignElements" sheetId="13" r:id="rId11"/>
+    <sheet name="configuration" sheetId="10" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="232">
   <si>
     <t>Epoch</t>
   </si>
@@ -65,9 +67,6 @@
     <t>Cycle End Rule</t>
   </si>
   <si>
-    <t>Visit Label</t>
-  </si>
-  <si>
     <t>Day 1</t>
   </si>
   <si>
@@ -83,9 +82,6 @@
     <t>EOT Visit</t>
   </si>
   <si>
-    <t>Visit Window</t>
-  </si>
-  <si>
     <t>-2..2 Days</t>
   </si>
   <si>
@@ -161,9 +157,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>BC/Profile</t>
-  </si>
-  <si>
     <t>studyTitle</t>
   </si>
   <si>
@@ -230,9 +223,6 @@
     <t>Active</t>
   </si>
   <si>
-    <t>cell</t>
-  </si>
-  <si>
     <t>Placebo</t>
   </si>
   <si>
@@ -573,13 +563,193 @@
   </si>
   <si>
     <t>Multiple cycles test</t>
+  </si>
+  <si>
+    <t>encounterName</t>
+  </si>
+  <si>
+    <t>encounterDescription</t>
+  </si>
+  <si>
+    <t>encounterType</t>
+  </si>
+  <si>
+    <t>encounterEnvironmentalSetting</t>
+  </si>
+  <si>
+    <t>encounterContactModes</t>
+  </si>
+  <si>
+    <t>transitionStartRule</t>
+  </si>
+  <si>
+    <t>transitionEndRule</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>Screening encounter</t>
+  </si>
+  <si>
+    <t>Visit</t>
+  </si>
+  <si>
+    <t>CLINIC</t>
+  </si>
+  <si>
+    <t>In Person</t>
+  </si>
+  <si>
+    <t>Subject identifier</t>
+  </si>
+  <si>
+    <t>IEs passed</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>Radomized</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>HOME</t>
+  </si>
+  <si>
+    <t>TELEPHONE CALL</t>
+  </si>
+  <si>
+    <t>Encounter xref</t>
+  </si>
+  <si>
+    <t>Window</t>
+  </si>
+  <si>
+    <t>BC/Procedure/Timeline</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
+    <t>E10</t>
+  </si>
+  <si>
+    <t>E11</t>
+  </si>
+  <si>
+    <t>Cycle 1, Day 1</t>
+  </si>
+  <si>
+    <t>Cycle 1, Day 15</t>
+  </si>
+  <si>
+    <t>Cycle 2, Day 1</t>
+  </si>
+  <si>
+    <t>Cycle 2, Day 15</t>
+  </si>
+  <si>
+    <t>Cycle 3, Day 1</t>
+  </si>
+  <si>
+    <t>Cycle 3, Day 15</t>
+  </si>
+  <si>
+    <t>Cycle 4 to 12, Day 1</t>
+  </si>
+  <si>
+    <t>Cycle 13 onwards, Day 15</t>
+  </si>
+  <si>
+    <t>End of Treatment Visit</t>
+  </si>
+  <si>
+    <t>Follow Up Visit</t>
+  </si>
+  <si>
+    <t>End of treatment</t>
+  </si>
+  <si>
+    <t>studyElementName</t>
+  </si>
+  <si>
+    <t>studyElementDescription</t>
+  </si>
+  <si>
+    <t>EL1</t>
+  </si>
+  <si>
+    <t>Screening Element</t>
+  </si>
+  <si>
+    <t>Study Start</t>
+  </si>
+  <si>
+    <t>Screened</t>
+  </si>
+  <si>
+    <t>EL2</t>
+  </si>
+  <si>
+    <t>EL3</t>
+  </si>
+  <si>
+    <t>Follow Up</t>
+  </si>
+  <si>
+    <t>Follow Up Element</t>
+  </si>
+  <si>
+    <t>Treated</t>
+  </si>
+  <si>
+    <t>Leave Study</t>
+  </si>
+  <si>
+    <t>Treatment Element</t>
+  </si>
+  <si>
+    <t>Completed treatment</t>
+  </si>
+  <si>
+    <t>studyDesignName</t>
+  </si>
+  <si>
+    <t>studyDesignDescription</t>
+  </si>
+  <si>
+    <t>Epoch/Arms</t>
+  </si>
+  <si>
+    <t>Study Design 1</t>
+  </si>
+  <si>
+    <t>The main design for the study</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -618,6 +788,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -645,7 +821,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -658,12 +834,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -703,17 +873,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -724,8 +885,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -738,6 +900,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1068,135 +1236,135 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="14" t="s">
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B9" s="17" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+      <c r="C9" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B5" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+      <c r="D9" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="B6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+      <c r="E9" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="F9" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="G9" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="H9" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="E9" s="20" t="s">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="B10" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="C10" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="D10" s="16" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>137</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="21">
+      <c r="G10" s="19">
         <v>40179</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="B11" s="18" t="s">
+      <c r="A11" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>135</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>139</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G11" s="21">
+        <v>136</v>
+      </c>
+      <c r="G11" s="19">
         <v>40544</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1205,6 +1373,377 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4154CB4E-EAA7-494D-AF71-EA9F1872735B}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="16" style="3" customWidth="1"/>
+    <col min="3" max="3" width="26" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" style="3" customWidth="1"/>
+    <col min="6" max="8" width="27.33203125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>196</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>197</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>199</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>200</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>201</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020DE536-FA14-3149-8856-3933D89EC48F}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="3" width="24.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="23.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{329FB390-8E4D-2044-99CB-68022604372C}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1218,19 +1757,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
-        <v>147</v>
+      <c r="A1" s="11" t="s">
+        <v>143</v>
       </c>
       <c r="B1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
-        <v>147</v>
+      <c r="A2" s="11" t="s">
+        <v>143</v>
       </c>
       <c r="B2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1253,43 +1792,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="F1" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="D2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>64</v>
+      <c r="F2" s="7" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1299,176 +1838,202 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B66121-AE3C-4E48-906B-C59A3DAEA708}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E3"/>
+      <selection activeCell="B10" sqref="B10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
+        <v>227</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>175</v>
-      </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>54</v>
+      <c r="A2" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+    </row>
+    <row r="3" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
+        <v>49</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C3" s="32"/>
       <c r="D3" s="32"/>
       <c r="E3" s="32"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="C12" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="31" t="s">
-        <v>145</v>
-      </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="31" t="s">
-        <v>146</v>
-      </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B7" s="31" t="s">
-        <v>153</v>
-      </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10" t="s">
+      <c r="B13" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
+      <c r="B14" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B6:E6"/>
+  <mergeCells count="10">
+    <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1482,14 +2047,14 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" style="1" customWidth="1"/>
     <col min="5" max="8" width="10.83203125" style="1"/>
     <col min="9" max="9" width="13" style="1" customWidth="1"/>
@@ -1500,438 +2065,438 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
-        <v>155</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="A1" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
       <c r="N1" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="A2" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="34">
+        <v>35</v>
+      </c>
+      <c r="E2" s="30">
         <v>1</v>
       </c>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34">
+      <c r="F2" s="30"/>
+      <c r="G2" s="30">
         <v>2</v>
       </c>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34">
+      <c r="H2" s="30"/>
+      <c r="I2" s="30">
         <v>3</v>
       </c>
-      <c r="J2" s="34"/>
+      <c r="J2" s="30"/>
       <c r="K2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="30"/>
+      <c r="K3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="30"/>
+      <c r="K4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="29"/>
+      <c r="K5" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>160</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="34"/>
-      <c r="K3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="34"/>
-      <c r="K4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="33"/>
-      <c r="K5" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="N6" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="6" t="s">
-        <v>6</v>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="21" t="s">
+        <v>193</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>1</v>
+        <v>179</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>8</v>
+        <v>186</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>187</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>8</v>
+        <v>189</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>8</v>
+        <v>196</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>7</v>
+        <v>198</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="M7" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="6" t="s">
+      <c r="G8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="N8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="C10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="C11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="C12" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="51" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1950,6 +2515,7 @@
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="I4:J4"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="57" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -1970,73 +2536,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>69</v>
+      <c r="A1" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>72</v>
+        <v>67</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>76</v>
+        <v>67</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" t="s">
         <v>73</v>
-      </c>
-      <c r="C5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2062,71 +2628,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>78</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>85</v>
+        <v>80</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>81</v>
       </c>
       <c r="E2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
       <c r="C3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>88</v>
-      </c>
       <c r="E3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B4">
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>91</v>
+        <v>80</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="E4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2149,46 +2715,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="B1" s="15" t="s">
+      <c r="A1" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="15" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="E1" s="15" t="s">
+      <c r="C2" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="D2" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G2" s="10" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2215,55 +2781,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="G1" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="D1" s="17" t="s">
+      <c r="H1" s="15" t="s">
         <v>104</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" t="s">
         <v>109</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
         <v>110</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>111</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>112</v>
-      </c>
-      <c r="E2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G2" t="s">
-        <v>115</v>
-      </c>
-      <c r="H2" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2284,58 +2850,58 @@
     <col min="1" max="1" width="7.33203125" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="24" style="29" customWidth="1"/>
+    <col min="4" max="4" width="24" style="24" customWidth="1"/>
     <col min="5" max="5" width="29.6640625" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>164</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>165</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>166</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>167</v>
+      <c r="A1" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D3" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="C3" t="s">
-        <v>172</v>
-      </c>
-      <c r="D3" s="29" t="s">
-        <v>173</v>
-      </c>
       <c r="E3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="7"/>
+      <c r="B5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>